<commit_message>
Refactor ExcelManager and CableComAppManager
</commit_message>
<xml_diff>
--- a/output/output.xlsx
+++ b/output/output.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/04ef7c6c9ce6ee46/Documents/GitHub/pole-permit-spreadsheet/output/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="11_01F1E2751B34F48A8853E5D0054BCD30BA3EDF80" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="11_20FBE2751B34F48A88E3E4811169D7308A36861B" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="65">
   <si>
     <t>Wireline Joint Use - Appendix A</t>
   </si>
@@ -122,13 +122,6 @@
     <t>PSE</t>
   </si>
   <si>
-    <t>nan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nan
-</t>
-  </si>
-  <si>
     <t>pse_primary_riser: 3311</t>
   </si>
   <si>
@@ -138,8 +131,7 @@
     <t>452654-156957</t>
   </si>
   <si>
-    <t>nan
-VIOLATION-catv is 27" from drip_loop
+    <t>VIOLATION-catv is 27" from drip_loop
 VIOLATION-catv is 21" from streetlight
 VIOLATION-fiber is 36" from streetlight</t>
   </si>
@@ -150,11 +142,13 @@
     <t>3-1</t>
   </si>
   <si>
+    <t>nan</t>
+  </si>
+  <si>
     <t>Distribution</t>
   </si>
   <si>
-    <t>nan
-VIOLATION-fiber is 29" from drip_loop
+    <t>VIOLATION-fiber is 29" from drip_loop
 VIOLATION-catv is 39" from drip_loop
 VIOLATION-catv is 10" from fiber
 VIOLATION-catv second attach is 5" from catv
@@ -171,16 +165,14 @@
     <t>452594-156957</t>
   </si>
   <si>
-    <t>nan
-VIOLATION-fiber is 24" from drip_loop
+    <t>VIOLATION-fiber is 24" from drip_loop
 VIOLATION-catv is 37" from drip_loop</t>
   </si>
   <si>
     <t>5-1</t>
   </si>
   <si>
-    <t>nan
-VIOLATION-fiber is 39" from neutral_height
+    <t>VIOLATION-fiber is 39" from neutral_height
 VIOLATION-fiber is 39" from secondary_spool
 VIOLATION-fiber is 31" from secondary_riser
 VIOLATION-fiber is 30" from drip_loop
@@ -193,8 +185,7 @@
     <t>452550-156955</t>
   </si>
   <si>
-    <t>nan
-VIOLATION-fiber is 26" from drip_loop
+    <t>VIOLATION-fiber is 26" from drip_loop
 VIOLATION-catv is 35" from drip_loop
 VIOLATION-catv is 9" from fiber</t>
   </si>
@@ -205,8 +196,7 @@
     <t>452525-156956</t>
   </si>
   <si>
-    <t>nan
-VIOLATION-catv is 11" from fiber</t>
+    <t>VIOLATION-catv is 11" from fiber</t>
   </si>
   <si>
     <t>8-1</t>
@@ -215,8 +205,7 @@
     <t>452499-156952</t>
   </si>
   <si>
-    <t>nan
-VIOLATION-fiber is 39" from drip_loop
+    <t>VIOLATION-fiber is 39" from drip_loop
 VIOLATION-catv is 6" from fiber
 VIOLATION-telco is 11" from fiber
 VIOLATION-telco is 5" from catv</t>
@@ -228,8 +217,7 @@
     <t>452485-156949</t>
   </si>
   <si>
-    <t>nan
-VIOLATION-catv is 30" from secondary_riser
+    <t>VIOLATION-catv is 30" from secondary_riser
 VIOLATION-telco is 37" from secondary_riser
 VIOLATION-catv is 28" from secondary_spool
 VIOLATION-telco is 35" from secondary_spool
@@ -837,8 +825,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="F4" workbookViewId="0">
-      <selection activeCell="Q11" sqref="Q11"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="R11" sqref="R11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1134,15 +1122,9 @@
       <c r="D10" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="E10" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="F10" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="G10" s="15" t="s">
-        <v>33</v>
-      </c>
+      <c r="E10" s="16"/>
+      <c r="F10" s="16"/>
+      <c r="G10" s="15"/>
       <c r="H10" s="17">
         <v>3400</v>
       </c>
@@ -1164,22 +1146,18 @@
       <c r="P10" s="17">
         <v>2701</v>
       </c>
-      <c r="Q10" s="23" t="s">
-        <v>34</v>
-      </c>
-      <c r="R10" s="18" t="s">
+      <c r="Q10" s="23"/>
+      <c r="R10" s="18"/>
+      <c r="S10" s="23" t="s">
         <v>33</v>
-      </c>
-      <c r="S10" s="23" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B11" s="21" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C11" s="14" t="s">
         <v>31</v>
@@ -1187,15 +1165,9 @@
       <c r="D11" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="E11" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="F11" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="G11" s="15" t="s">
-        <v>33</v>
-      </c>
+      <c r="E11" s="16"/>
+      <c r="F11" s="16"/>
+      <c r="G11" s="15"/>
       <c r="H11" s="17">
         <v>2808</v>
       </c>
@@ -1220,37 +1192,29 @@
         <v>2305</v>
       </c>
       <c r="Q11" s="23" t="s">
-        <v>38</v>
-      </c>
-      <c r="R11" s="18" t="s">
-        <v>33</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="R11" s="18"/>
       <c r="S11" s="23" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="B12" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="C12" s="14" t="s">
         <v>40</v>
-      </c>
-      <c r="B12" s="21" t="s">
-        <v>33</v>
-      </c>
-      <c r="C12" s="14" t="s">
-        <v>41</v>
       </c>
       <c r="D12" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="E12" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="F12" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="G12" s="15" t="s">
-        <v>33</v>
-      </c>
+      <c r="E12" s="16"/>
+      <c r="F12" s="16"/>
+      <c r="G12" s="15"/>
       <c r="H12" s="17">
         <v>2702</v>
       </c>
@@ -1275,37 +1239,29 @@
         <v>2304</v>
       </c>
       <c r="Q12" s="23" t="s">
+        <v>41</v>
+      </c>
+      <c r="R12" s="18"/>
+      <c r="S12" s="23" t="s">
         <v>42</v>
-      </c>
-      <c r="R12" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="S12" s="23" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="B13" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="B13" s="21" t="s">
-        <v>45</v>
-      </c>
       <c r="C13" s="14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D13" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="E13" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="F13" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="G13" s="15" t="s">
-        <v>33</v>
-      </c>
+      <c r="E13" s="16"/>
+      <c r="F13" s="16"/>
+      <c r="G13" s="15"/>
       <c r="H13" s="17">
         <v>2500</v>
       </c>
@@ -1330,37 +1286,29 @@
         <v>2102</v>
       </c>
       <c r="Q13" s="23" t="s">
-        <v>46</v>
-      </c>
-      <c r="R13" s="18" t="s">
-        <v>33</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="R13" s="18"/>
       <c r="S13" s="23" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="13" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B14" s="21" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D14" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="E14" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="F14" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="G14" s="15" t="s">
-        <v>33</v>
-      </c>
+      <c r="E14" s="16"/>
+      <c r="F14" s="16"/>
+      <c r="G14" s="15"/>
       <c r="H14" s="17">
         <v>2608</v>
       </c>
@@ -1387,37 +1335,29 @@
         <v>2305</v>
       </c>
       <c r="Q14" s="23" t="s">
-        <v>48</v>
-      </c>
-      <c r="R14" s="18" t="s">
-        <v>33</v>
-      </c>
+        <v>47</v>
+      </c>
+      <c r="R14" s="18"/>
       <c r="S14" s="23" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="B15" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="B15" s="21" t="s">
-        <v>50</v>
-      </c>
       <c r="C15" s="14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D15" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="E15" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="F15" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="G15" s="15" t="s">
-        <v>33</v>
-      </c>
+      <c r="E15" s="16"/>
+      <c r="F15" s="16"/>
+      <c r="G15" s="15"/>
       <c r="H15" s="17">
         <v>3008</v>
       </c>
@@ -1442,37 +1382,29 @@
         <v>2606</v>
       </c>
       <c r="Q15" s="23" t="s">
-        <v>51</v>
-      </c>
-      <c r="R15" s="18" t="s">
-        <v>33</v>
-      </c>
+        <v>50</v>
+      </c>
+      <c r="R15" s="18"/>
       <c r="S15" s="23" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="B16" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="B16" s="21" t="s">
-        <v>53</v>
-      </c>
       <c r="C16" s="14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D16" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="E16" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="F16" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="G16" s="15" t="s">
-        <v>33</v>
-      </c>
+      <c r="E16" s="16"/>
+      <c r="F16" s="16"/>
+      <c r="G16" s="15"/>
       <c r="H16" s="17">
         <v>3006</v>
       </c>
@@ -1499,37 +1431,29 @@
         <v>2403</v>
       </c>
       <c r="Q16" s="23" t="s">
-        <v>54</v>
-      </c>
-      <c r="R16" s="18" t="s">
-        <v>33</v>
-      </c>
+        <v>53</v>
+      </c>
+      <c r="R16" s="18"/>
       <c r="S16" s="23" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
     </row>
     <row r="17" spans="1:19" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="B17" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="B17" s="21" t="s">
-        <v>56</v>
-      </c>
       <c r="C17" s="14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D17" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="E17" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="F17" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="G17" s="15" t="s">
-        <v>33</v>
-      </c>
+      <c r="E17" s="16"/>
+      <c r="F17" s="16"/>
+      <c r="G17" s="15"/>
       <c r="H17" s="17">
         <v>2910</v>
       </c>
@@ -1554,37 +1478,29 @@
         <v>2511</v>
       </c>
       <c r="Q17" s="23" t="s">
-        <v>57</v>
-      </c>
-      <c r="R17" s="18" t="s">
-        <v>33</v>
-      </c>
+        <v>56</v>
+      </c>
+      <c r="R17" s="18"/>
       <c r="S17" s="23" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
     </row>
     <row r="18" spans="1:19" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="B18" s="21" t="s">
         <v>58</v>
       </c>
-      <c r="B18" s="21" t="s">
-        <v>59</v>
-      </c>
       <c r="C18" s="14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D18" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="E18" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="F18" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="G18" s="15" t="s">
-        <v>33</v>
-      </c>
+      <c r="E18" s="16"/>
+      <c r="F18" s="16"/>
+      <c r="G18" s="15"/>
       <c r="H18" s="17"/>
       <c r="I18" s="17">
         <v>2508</v>
@@ -1605,13 +1521,11 @@
       <c r="O18" s="17"/>
       <c r="P18" s="17"/>
       <c r="Q18" s="23" t="s">
-        <v>60</v>
-      </c>
-      <c r="R18" s="18" t="s">
-        <v>33</v>
-      </c>
+        <v>59</v>
+      </c>
+      <c r="R18" s="18"/>
       <c r="S18" s="23" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
     </row>
     <row r="19" spans="1:19" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -4970,7 +4884,7 @@
   <sheetData>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="20" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C2" s="20" t="s">
         <v>32</v>
@@ -4981,23 +4895,23 @@
         <v>31</v>
       </c>
       <c r="C3" s="20" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="C4" s="20" t="s">
         <v>62</v>
-      </c>
-      <c r="C4" s="20" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="20" t="s">
+        <v>63</v>
+      </c>
+      <c r="C5" s="20" t="s">
         <v>64</v>
-      </c>
-      <c r="C5" s="20" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Make ready with proposed values
</commit_message>
<xml_diff>
--- a/output/output.xlsx
+++ b/output/output.xlsx
@@ -1169,7 +1169,8 @@
       <c r="P11" s="17" t="n"/>
       <c r="Q11" s="23" t="inlineStr">
         <is>
-          <t>VIOLATION-catv is 27" from drip_loop</t>
+          <t>Dress Drip Loop
+Ground Streetlight</t>
         </is>
       </c>
       <c r="R11" s="18" t="inlineStr">
@@ -1184,12 +1185,12 @@
       </c>
       <c r="T11" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="U11" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -1252,11 +1253,8 @@
       <c r="P12" s="17" t="n"/>
       <c r="Q12" s="23" t="inlineStr">
         <is>
-          <t>VIOLATION-fiber is 29" from drip_loop
-VIOLATION-catv is 39" from drip_loop
-VIOLATION-catv is 10" from fiber
-VIOLATION-catv second attach is 5" from catv
-VIOLATION-telco is 8" from telco second attach</t>
+          <t>Dress Drip Loop
+Move CATV to: 22' 04"</t>
         </is>
       </c>
       <c r="R12" s="18" t="inlineStr">
@@ -1340,8 +1338,7 @@
       <c r="P13" s="17" t="n"/>
       <c r="Q13" s="23" t="inlineStr">
         <is>
-          <t>VIOLATION-fiber is 24" from drip_loop
-VIOLATION-catv is 37" from drip_loop</t>
+          <t>Dress Drip Loop</t>
         </is>
       </c>
       <c r="R13" s="18" t="inlineStr">
@@ -1415,10 +1412,10 @@
       </c>
       <c r="L14" s="17" t="n"/>
       <c r="M14" s="17" t="n">
+        <v>2206</v>
+      </c>
+      <c r="N14" s="17" t="n">
         <v>2106</v>
-      </c>
-      <c r="N14" s="17" t="n">
-        <v>2206</v>
       </c>
       <c r="O14" s="17" t="n">
         <v>2305</v>
@@ -1426,11 +1423,9 @@
       <c r="P14" s="17" t="n"/>
       <c r="Q14" s="23" t="inlineStr">
         <is>
-          <t>VIOLATION-fiber is 39" from neutral_height
-VIOLATION-fiber is 39" from secondary_spool
-VIOLATION-fiber is 31" from secondary_riser
-VIOLATION-fiber is 30" from drip_loop
-VIOLATION-telco is 11" from fiber</t>
+          <t>Move Fiber to: 22' 06"
+Move CATV to: 21' 06"
+Move TelCo to: 20' 06"</t>
         </is>
       </c>
       <c r="R14" s="18" t="inlineStr">
@@ -1513,9 +1508,8 @@
       <c r="P15" s="17" t="n"/>
       <c r="Q15" s="23" t="inlineStr">
         <is>
-          <t>VIOLATION-fiber is 26" from drip_loop
-VIOLATION-catv is 35" from drip_loop
-VIOLATION-catv is 9" from fiber</t>
+          <t>Dress Drip Loop
+Move Fiber to: 26' 10"</t>
         </is>
       </c>
       <c r="R15" s="18" t="inlineStr">
@@ -1600,7 +1594,7 @@
       <c r="P16" s="17" t="n"/>
       <c r="Q16" s="23" t="inlineStr">
         <is>
-          <t>VIOLATION-catv is 11" from fiber</t>
+          <t>Move CATV to: 23' 00"</t>
         </is>
       </c>
       <c r="R16" s="18" t="inlineStr">
@@ -1683,10 +1677,9 @@
       <c r="P17" s="17" t="n"/>
       <c r="Q17" s="23" t="inlineStr">
         <is>
-          <t>VIOLATION-fiber is 39" from drip_loop
-VIOLATION-catv is 6" from fiber
-VIOLATION-telco is 11" from fiber
-VIOLATION-telco is 5" from catv</t>
+          <t>Dress Drip Loop
+Move CATV to: 24' 11"
+Move TelCo to: 23' 11"</t>
         </is>
       </c>
       <c r="R17" s="18" t="inlineStr">
@@ -1767,13 +1760,8 @@
       <c r="P18" s="17" t="n"/>
       <c r="Q18" s="23" t="inlineStr">
         <is>
-          <t>VIOLATION-catv is 30" from secondary_riser
-VIOLATION-telco is 37" from secondary_riser
-VIOLATION-catv is 28" from secondary_spool
-VIOLATION-telco is 35" from secondary_spool
-VIOLATION-catv is 20" from drip_loop
-VIOLATION-telco is 27" from drip_loop
-VIOLATION-telco is 7" from catv</t>
+          <t>Move CATV to: 21' 08"
+Move TelCo to: 20' 08"</t>
         </is>
       </c>
       <c r="R18" s="18" t="inlineStr">

</xml_diff>